<commit_message>
Ajoute des entêtes colorées dans les colonnes non-obligatoire du template de service V2
</commit_message>
<xml_diff>
--- a/public/assets/fichiers/Template services v2 - MSS.xlsx
+++ b/public/assets/fichiers/Template services v2 - MSS.xlsx
@@ -261,7 +261,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +278,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0079D0"/>
         <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6FA8DC"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -358,7 +364,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,15 +485,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,7 +548,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFAFABAB"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF6FA8DC"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFEFEFEF"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -590,9 +604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1928520</xdr:colOff>
+      <xdr:colOff>1928160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>813960</xdr:rowOff>
+      <xdr:rowOff>813600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -606,7 +620,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1928520" cy="813960"/>
+          <a:ext cx="1928160" cy="813600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -631,12 +645,12 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topRight" activeCell="T11" activeCellId="0" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="14.16"/>
@@ -646,7 +660,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="999" style="0" width="11.5"/>
   </cols>
@@ -836,52 +850,52 @@
       <c r="D6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="32" t="s">
+      <c r="R6" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -894,14 +908,14 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="20"/>
-      <c r="O7" s="34"/>
+      <c r="O7" s="36"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -914,14 +928,14 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
-      <c r="O8" s="34"/>
+      <c r="O8" s="36"/>
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -934,14 +948,14 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
-      <c r="O9" s="35"/>
+      <c r="O9" s="37"/>
       <c r="P9" s="20"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -954,14 +968,14 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
-      <c r="O10" s="34"/>
+      <c r="O10" s="36"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
@@ -974,14 +988,14 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
-      <c r="O11" s="35"/>
+      <c r="O11" s="37"/>
       <c r="P11" s="20"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -994,14 +1008,14 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="20"/>
-      <c r="O12" s="35"/>
+      <c r="O12" s="37"/>
       <c r="P12" s="20"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
@@ -1014,14 +1028,14 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
-      <c r="O13" s="35"/>
+      <c r="O13" s="37"/>
       <c r="P13" s="20"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -1034,14 +1048,14 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
-      <c r="O14" s="35"/>
+      <c r="O14" s="37"/>
       <c r="P14" s="20"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -1054,14 +1068,14 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
-      <c r="O15" s="35"/>
+      <c r="O15" s="37"/>
       <c r="P15" s="20"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1074,14 +1088,14 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
-      <c r="O16" s="35"/>
+      <c r="O16" s="37"/>
       <c r="P16" s="20"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -1094,14 +1108,14 @@
       <c r="L17" s="20"/>
       <c r="M17" s="20"/>
       <c r="N17" s="20"/>
-      <c r="O17" s="35"/>
+      <c r="O17" s="37"/>
       <c r="P17" s="20"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -1114,14 +1128,14 @@
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
-      <c r="O18" s="35"/>
+      <c r="O18" s="37"/>
       <c r="P18" s="20"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -1134,14 +1148,14 @@
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
       <c r="N19" s="20"/>
-      <c r="O19" s="35"/>
+      <c r="O19" s="37"/>
       <c r="P19" s="20"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -1154,14 +1168,14 @@
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
       <c r="N20" s="20"/>
-      <c r="O20" s="35"/>
+      <c r="O20" s="37"/>
       <c r="P20" s="20"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -1174,14 +1188,14 @@
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
       <c r="N21" s="20"/>
-      <c r="O21" s="35"/>
+      <c r="O21" s="37"/>
       <c r="P21" s="20"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="36"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -1194,14 +1208,14 @@
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
-      <c r="O22" s="35"/>
+      <c r="O22" s="37"/>
       <c r="P22" s="20"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="36"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -1214,14 +1228,14 @@
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
       <c r="N23" s="20"/>
-      <c r="O23" s="35"/>
+      <c r="O23" s="37"/>
       <c r="P23" s="20"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -1234,14 +1248,14 @@
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
       <c r="N24" s="20"/>
-      <c r="O24" s="35"/>
+      <c r="O24" s="37"/>
       <c r="P24" s="20"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="36"/>
-      <c r="B25" s="35"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -1254,14 +1268,14 @@
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
       <c r="N25" s="20"/>
-      <c r="O25" s="35"/>
+      <c r="O25" s="37"/>
       <c r="P25" s="20"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36"/>
-      <c r="B26" s="35"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -1274,14 +1288,14 @@
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="35"/>
+      <c r="O26" s="37"/>
       <c r="P26" s="20"/>
-      <c r="Q26" s="36"/>
-      <c r="R26" s="36"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="36"/>
-      <c r="B27" s="35"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -1294,14 +1308,14 @@
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
       <c r="N27" s="20"/>
-      <c r="O27" s="35"/>
+      <c r="O27" s="37"/>
       <c r="P27" s="20"/>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="36"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36"/>
-      <c r="B28" s="35"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -1314,14 +1328,14 @@
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
       <c r="N28" s="20"/>
-      <c r="O28" s="35"/>
+      <c r="O28" s="37"/>
       <c r="P28" s="20"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="36"/>
-      <c r="B29" s="35"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -1334,14 +1348,14 @@
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
       <c r="N29" s="20"/>
-      <c r="O29" s="35"/>
+      <c r="O29" s="37"/>
       <c r="P29" s="20"/>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="36"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="36"/>
-      <c r="B30" s="35"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
@@ -1354,10 +1368,10 @@
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
       <c r="N30" s="20"/>
-      <c r="O30" s="35"/>
+      <c r="O30" s="37"/>
       <c r="P30" s="20"/>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="36"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>